<commit_message>
Updated export to account for loss of Tetilla, and updated visualisation files
</commit_message>
<xml_diff>
--- a/data/dataPaper-I-in/arphified/Porifera.xlsx
+++ b/data/dataPaper-I-in/arphified/Porifera.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1686" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="427">
   <si>
     <t>Taxon_Local_ID</t>
   </si>
@@ -586,6 +586,12 @@
   </si>
   <si>
     <t>villosa</t>
+  </si>
+  <si>
+    <t>247194</t>
+  </si>
+  <si>
+    <t>Tetilla</t>
   </si>
   <si>
     <t>213993</t>
@@ -1664,7 +1670,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH40"/>
+  <dimension ref="A1:AH41"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
@@ -5226,43 +5232,43 @@
         <v>68</v>
       </c>
       <c r="H35" t="s">
+        <v>69</v>
+      </c>
+      <c r="I35" t="s">
+        <v>36</v>
+      </c>
+      <c r="J35" t="s">
+        <v>186</v>
+      </c>
+      <c r="K35" t="s">
+        <v>187</v>
+      </c>
+      <c r="L35" t="s">
+        <v>36</v>
+      </c>
+      <c r="M35" t="s">
+        <v>36</v>
+      </c>
+      <c r="N35" t="s">
+        <v>188</v>
+      </c>
+      <c r="O35" t="s">
+        <v>36</v>
+      </c>
+      <c r="P35" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>36</v>
+      </c>
+      <c r="R35" t="s">
         <v>192</v>
       </c>
-      <c r="I35" t="s">
-        <v>36</v>
-      </c>
-      <c r="J35" t="s">
-        <v>193</v>
-      </c>
-      <c r="K35" t="s">
-        <v>36</v>
-      </c>
-      <c r="L35" t="s">
-        <v>36</v>
-      </c>
-      <c r="M35" t="s">
-        <v>36</v>
-      </c>
-      <c r="N35" t="s">
-        <v>194</v>
-      </c>
-      <c r="O35" t="s">
-        <v>36</v>
-      </c>
-      <c r="P35" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q35" t="s">
-        <v>36</v>
-      </c>
-      <c r="R35" t="s">
-        <v>195</v>
-      </c>
       <c r="S35" t="s">
         <v>36</v>
       </c>
       <c r="T35" t="s">
-        <v>196</v>
+        <v>66</v>
       </c>
       <c r="U35" t="s">
         <v>36</v>
@@ -5274,7 +5280,7 @@
         <v>36</v>
       </c>
       <c r="X35" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="Y35" t="s">
         <v>36</v>
@@ -5309,7 +5315,7 @@
     </row>
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B36" t="s">
         <v>35</v>
@@ -5330,13 +5336,13 @@
         <v>68</v>
       </c>
       <c r="H36" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I36" t="s">
         <v>36</v>
       </c>
       <c r="J36" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="K36" t="s">
         <v>36</v>
@@ -5348,7 +5354,7 @@
         <v>36</v>
       </c>
       <c r="N36" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="O36" t="s">
         <v>36</v>
@@ -5360,13 +5366,13 @@
         <v>36</v>
       </c>
       <c r="R36" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="S36" t="s">
         <v>36</v>
       </c>
       <c r="T36" t="s">
-        <v>66</v>
+        <v>198</v>
       </c>
       <c r="U36" t="s">
         <v>36</v>
@@ -5378,7 +5384,7 @@
         <v>36</v>
       </c>
       <c r="X36" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="Y36" t="s">
         <v>36</v>
@@ -5413,7 +5419,7 @@
     </row>
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
@@ -5434,13 +5440,13 @@
         <v>68</v>
       </c>
       <c r="H37" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I37" t="s">
         <v>36</v>
       </c>
       <c r="J37" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="K37" t="s">
         <v>36</v>
@@ -5452,7 +5458,7 @@
         <v>36</v>
       </c>
       <c r="N37" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="O37" t="s">
         <v>36</v>
@@ -5464,7 +5470,7 @@
         <v>36</v>
       </c>
       <c r="R37" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="S37" t="s">
         <v>36</v>
@@ -5517,7 +5523,7 @@
     </row>
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B38" t="s">
         <v>35</v>
@@ -5535,46 +5541,46 @@
         <v>36</v>
       </c>
       <c r="G38" t="s">
+        <v>68</v>
+      </c>
+      <c r="H38" t="s">
+        <v>194</v>
+      </c>
+      <c r="I38" t="s">
+        <v>36</v>
+      </c>
+      <c r="J38" t="s">
+        <v>201</v>
+      </c>
+      <c r="K38" t="s">
+        <v>36</v>
+      </c>
+      <c r="L38" t="s">
+        <v>36</v>
+      </c>
+      <c r="M38" t="s">
+        <v>36</v>
+      </c>
+      <c r="N38" t="s">
+        <v>202</v>
+      </c>
+      <c r="O38" t="s">
+        <v>36</v>
+      </c>
+      <c r="P38" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>36</v>
+      </c>
+      <c r="R38" t="s">
         <v>203</v>
       </c>
-      <c r="H38" t="s">
-        <v>204</v>
-      </c>
-      <c r="I38" t="s">
-        <v>36</v>
-      </c>
-      <c r="J38" t="s">
-        <v>205</v>
-      </c>
-      <c r="K38" t="s">
-        <v>36</v>
-      </c>
-      <c r="L38" t="s">
-        <v>36</v>
-      </c>
-      <c r="M38" t="s">
-        <v>36</v>
-      </c>
-      <c r="N38" t="s">
-        <v>206</v>
-      </c>
-      <c r="O38" t="s">
-        <v>36</v>
-      </c>
-      <c r="P38" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q38" t="s">
-        <v>36</v>
-      </c>
-      <c r="R38" t="s">
-        <v>207</v>
-      </c>
       <c r="S38" t="s">
         <v>36</v>
       </c>
       <c r="T38" t="s">
-        <v>208</v>
+        <v>66</v>
       </c>
       <c r="U38" t="s">
         <v>36</v>
@@ -5586,7 +5592,7 @@
         <v>36</v>
       </c>
       <c r="X38" t="s">
-        <v>121</v>
+        <v>36</v>
       </c>
       <c r="Y38" t="s">
         <v>36</v>
@@ -5621,7 +5627,7 @@
     </row>
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="B39" t="s">
         <v>35</v>
@@ -5639,47 +5645,47 @@
         <v>36</v>
       </c>
       <c r="G39" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H39" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I39" t="s">
         <v>36</v>
       </c>
       <c r="J39" t="s">
+        <v>207</v>
+      </c>
+      <c r="K39" t="s">
+        <v>36</v>
+      </c>
+      <c r="L39" t="s">
+        <v>36</v>
+      </c>
+      <c r="M39" t="s">
+        <v>36</v>
+      </c>
+      <c r="N39" t="s">
+        <v>208</v>
+      </c>
+      <c r="O39" t="s">
+        <v>36</v>
+      </c>
+      <c r="P39" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>36</v>
+      </c>
+      <c r="R39" t="s">
+        <v>209</v>
+      </c>
+      <c r="S39" t="s">
+        <v>36</v>
+      </c>
+      <c r="T39" t="s">
         <v>210</v>
       </c>
-      <c r="K39" t="s">
-        <v>36</v>
-      </c>
-      <c r="L39" t="s">
-        <v>36</v>
-      </c>
-      <c r="M39" t="s">
-        <v>36</v>
-      </c>
-      <c r="N39" t="s">
-        <v>211</v>
-      </c>
-      <c r="O39" t="s">
-        <v>36</v>
-      </c>
-      <c r="P39" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q39" t="s">
-        <v>36</v>
-      </c>
-      <c r="R39" t="s">
-        <v>212</v>
-      </c>
-      <c r="S39" t="s">
-        <v>36</v>
-      </c>
-      <c r="T39" t="s">
-        <v>213</v>
-      </c>
       <c r="U39" t="s">
         <v>36</v>
       </c>
@@ -5690,7 +5696,7 @@
         <v>36</v>
       </c>
       <c r="X39" t="s">
-        <v>214</v>
+        <v>121</v>
       </c>
       <c r="Y39" t="s">
         <v>36</v>
@@ -5725,7 +5731,7 @@
     </row>
     <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B40" t="s">
         <v>35</v>
@@ -5743,16 +5749,16 @@
         <v>36</v>
       </c>
       <c r="G40" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H40" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="I40" t="s">
         <v>36</v>
       </c>
       <c r="J40" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="K40" t="s">
         <v>36</v>
@@ -5764,7 +5770,7 @@
         <v>36</v>
       </c>
       <c r="N40" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="O40" t="s">
         <v>36</v>
@@ -5776,54 +5782,158 @@
         <v>36</v>
       </c>
       <c r="R40" t="s">
+        <v>214</v>
+      </c>
+      <c r="S40" t="s">
+        <v>36</v>
+      </c>
+      <c r="T40" t="s">
+        <v>215</v>
+      </c>
+      <c r="U40" t="s">
+        <v>36</v>
+      </c>
+      <c r="V40" t="s">
+        <v>36</v>
+      </c>
+      <c r="W40" t="s">
+        <v>36</v>
+      </c>
+      <c r="X40" t="s">
         <v>216</v>
       </c>
-      <c r="S40" t="s">
-        <v>36</v>
-      </c>
-      <c r="T40" t="s">
+      <c r="Y40" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG40" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH40" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>217</v>
       </c>
-      <c r="U40" t="s">
-        <v>36</v>
-      </c>
-      <c r="V40" t="s">
-        <v>36</v>
-      </c>
-      <c r="W40" t="s">
-        <v>36</v>
-      </c>
-      <c r="X40" t="s">
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="C41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F41" t="s">
+        <v>36</v>
+      </c>
+      <c r="G41" t="s">
+        <v>205</v>
+      </c>
+      <c r="H41" t="s">
+        <v>206</v>
+      </c>
+      <c r="I41" t="s">
+        <v>36</v>
+      </c>
+      <c r="J41" t="s">
+        <v>212</v>
+      </c>
+      <c r="K41" t="s">
+        <v>36</v>
+      </c>
+      <c r="L41" t="s">
+        <v>36</v>
+      </c>
+      <c r="M41" t="s">
+        <v>36</v>
+      </c>
+      <c r="N41" t="s">
+        <v>213</v>
+      </c>
+      <c r="O41" t="s">
+        <v>36</v>
+      </c>
+      <c r="P41" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>36</v>
+      </c>
+      <c r="R41" t="s">
         <v>218</v>
       </c>
-      <c r="Y40" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG40" t="s">
-        <v>36</v>
-      </c>
-      <c r="AH40" t="s">
+      <c r="S41" t="s">
+        <v>36</v>
+      </c>
+      <c r="T41" t="s">
+        <v>219</v>
+      </c>
+      <c r="U41" t="s">
+        <v>36</v>
+      </c>
+      <c r="V41" t="s">
+        <v>36</v>
+      </c>
+      <c r="W41" t="s">
+        <v>36</v>
+      </c>
+      <c r="X41" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG41" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH41" t="s">
         <v>36</v>
       </c>
     </row>
@@ -5843,495 +5953,495 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C1" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D1" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E1" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F1" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="G1" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="H1" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="I1" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="J1" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="L1" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="M1" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="N1" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="O1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="P1" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="Q1" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="R1" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="S1" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="T1" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="U1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="V1" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="W1" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="X1" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="Y1" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="Z1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="AA1" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="AB1" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="AC1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="AD1" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="AE1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="AF1" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="AG1" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="AH1" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="AI1" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="AJ1" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="AK1" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="AL1" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="AM1" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="AN1" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="AO1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="AP1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="AQ1" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="AR1" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="AS1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="AT1" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AU1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="AV1" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="AW1" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="AX1" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="AY1" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AZ1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="BA1" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="BB1" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="BC1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="BD1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="BE1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="BF1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="BG1" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="BH1" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="BI1" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="BJ1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="BK1" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="BL1" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="BM1" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="BN1" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="BO1" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="BP1" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="BQ1" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="BR1" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="BS1" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="BT1" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="BU1" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="BV1" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="BW1" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="BX1" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="BY1" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="BZ1" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="CA1" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="CB1" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="CC1" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="CD1" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="CE1" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="CF1" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="CG1" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="CH1" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="CI1" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="CJ1" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="CK1" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="CL1" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="CM1" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="CN1" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="CO1" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="CP1" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="CQ1" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="CR1" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="CS1" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="CT1" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="CU1" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="CV1" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="CW1" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="CX1" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="CY1" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="CZ1" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="DA1" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="DB1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="DC1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="DD1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="DE1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="DF1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="DG1" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="DH1" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="DI1" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="DJ1" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="DK1" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="DL1" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="DM1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="DN1" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="DO1" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="DP1" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="DQ1" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="DR1" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="DS1" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="DT1" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="DU1" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="DV1" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="DW1" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="DX1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="DY1" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="DZ1" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="EA1" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="EB1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="EC1" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="ED1" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="EE1" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="EF1" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="EG1" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="EH1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="EI1" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="EJ1" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="EK1" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="EL1" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="EM1" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="EN1" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="EO1" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="EP1" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="EQ1" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="ER1" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="ES1" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="ET1" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="EU1" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="EV1" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="EW1" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="EX1" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="EY1" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="EZ1" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="FA1" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="FB1" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="FC1" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="FD1" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="2" spans="1:160" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B2" t="s">
         <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="D2" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="E2" t="s">
         <v>36</v>
@@ -6343,428 +6453,428 @@
         <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="I2" t="s">
         <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="K2" t="s">
+        <v>385</v>
+      </c>
+      <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>36</v>
+      </c>
+      <c r="N2" t="s">
+        <v>36</v>
+      </c>
+      <c r="O2" t="s">
+        <v>36</v>
+      </c>
+      <c r="P2" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>387</v>
+      </c>
+      <c r="U2" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" t="s">
+        <v>388</v>
+      </c>
+      <c r="W2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>389</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>390</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>391</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>392</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>393</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>394</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>395</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>396</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>397</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>398</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>399</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>400</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>401</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>402</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>403</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>404</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>405</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>406</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>407</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>408</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>409</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>410</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CT2" t="s">
         <v>383</v>
       </c>
-      <c r="L2" t="s">
-        <v>36</v>
-      </c>
-      <c r="M2" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" t="s">
-        <v>384</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" t="s">
-        <v>385</v>
-      </c>
-      <c r="U2" t="s">
-        <v>36</v>
-      </c>
-      <c r="V2" t="s">
-        <v>386</v>
-      </c>
-      <c r="W2" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>387</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG2" t="s">
+      <c r="CU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>411</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>412</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>413</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>414</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>415</v>
+      </c>
+      <c r="EE2" t="s">
+        <v>416</v>
+      </c>
+      <c r="EF2" t="s">
+        <v>417</v>
+      </c>
+      <c r="EG2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EH2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EI2" t="s">
+        <v>418</v>
+      </c>
+      <c r="EJ2" t="s">
+        <v>419</v>
+      </c>
+      <c r="EK2" t="s">
+        <v>420</v>
+      </c>
+      <c r="EL2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EM2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EN2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EO2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EP2" t="s">
+        <v>36</v>
+      </c>
+      <c r="EQ2" t="s">
+        <v>36</v>
+      </c>
+      <c r="ER2" t="s">
         <v>388</v>
       </c>
-      <c r="AH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>389</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>390</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>391</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>392</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>393</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>394</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>395</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>396</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>397</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>398</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>399</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>400</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>401</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>402</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>403</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>404</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>405</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>406</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>407</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>408</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>381</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>409</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>410</v>
-      </c>
-      <c r="DY2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DZ2" t="s">
-        <v>411</v>
-      </c>
-      <c r="EA2" t="s">
-        <v>412</v>
-      </c>
-      <c r="EB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EC2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ED2" t="s">
-        <v>413</v>
-      </c>
-      <c r="EE2" t="s">
-        <v>414</v>
-      </c>
-      <c r="EF2" t="s">
-        <v>415</v>
-      </c>
-      <c r="EG2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EH2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EI2" t="s">
-        <v>416</v>
-      </c>
-      <c r="EJ2" t="s">
-        <v>417</v>
-      </c>
-      <c r="EK2" t="s">
-        <v>418</v>
-      </c>
-      <c r="EL2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EM2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EO2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EP2" t="s">
-        <v>36</v>
-      </c>
-      <c r="EQ2" t="s">
-        <v>36</v>
-      </c>
-      <c r="ER2" t="s">
-        <v>386</v>
-      </c>
       <c r="ES2" t="s">
         <v>36</v>
       </c>
@@ -6775,19 +6885,19 @@
         <v>36</v>
       </c>
       <c r="EV2" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="EW2" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="EX2" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="EY2" t="s">
         <v>36</v>
       </c>
       <c r="EZ2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="FA2" t="s">
         <v>36</v>
@@ -6818,10 +6928,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C1" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>